<commit_message>
Projenin tüm dosyaları eklendi
</commit_message>
<xml_diff>
--- a/outputs/excel_raporlar/sohbet_analiz.xlsx
+++ b/outputs/excel_raporlar/sohbet_analiz.xlsx
@@ -615,7 +615,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Siparişte eksik ürün olması ve çözüm talebi</t>
+          <t>Siparişte eksik ürün bildirimi</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -673,9 +673,9 @@
           <t>Negatif</t>
         </is>
       </c>
-      <c r="G3" s="4" t="inlineStr">
-        <is>
-          <t>Şikayet</t>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Sorun</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
@@ -888,14 +888,14 @@
           <t>İstek</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t>İade</t>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>İptal</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Sipariş iptali ve iade süreci</t>
+          <t>Sipariş iptali</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1030,12 +1030,12 @@
       </c>
       <c r="H8" s="4" t="inlineStr">
         <is>
-          <t>İade</t>
+          <t>Hasarlı ürün</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Defolu ürün için iade/değişim talebi; fotoğraf kanıtı istemine karşı direniş</t>
+          <t>Defolu ürün için iade/değişim talebi, fotoğraf kanıtı gerektiği konusunda memnuniyetsizlik</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Profil bilgilerini güncelleme</t>
+          <t>Üyelik bilgilerimi güncellemek</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Fatura üzerindeki hatalı fiyatın düzeltilmesi ve yeni faturanın gönderilmesi</t>
+          <t>Fatura üzerinde hatalı fiyatlar tespiti ve düzeltme talebi</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Sipariş iptalinin sistemde yapılamaması ve iade süreciyle devam etmek zorunda kalınması</t>
+          <t>İptal butonunun görünmemesi ve iptal edilememesi nedeniyle hizmetten memnuniyetsizlik</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Stok bilgisi ve gelecek stok tarihi talebi</t>
+          <t>Ürün stok durumu ve stok gelecekteki geliş tarihi bilgisi</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1373,19 +1373,19 @@
           <t>Negatif</t>
         </is>
       </c>
-      <c r="G13" s="3" t="inlineStr">
-        <is>
-          <t>Şikayet</t>
-        </is>
-      </c>
-      <c r="H13" s="4" t="inlineStr">
-        <is>
-          <t>Kargo</t>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Sorun</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>Ödeme</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Çift çekim/ödemeyle ilgili sorun</t>
+          <t>Kredi kartı iki kez çekim işlemi (çekim hatası)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1503,9 +1503,9 @@
           <t>0 dk 40 sn</t>
         </is>
       </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>Çözülemedi</t>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
+          <t>Çözüldü</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Kredi kartı reddedilmesi</t>
+          <t>Kredi kartı reddediliyor</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Ürün beden tablosu bilgisi arandı</t>
+          <t>Ürün beden tablosu bilgisini bulma</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Yanlış adres girdim, düzeltme yöntemine yönelik sorun</t>
+          <t>Adres yanlış girdim ve düzeltme yolu soruldu fakat çözüm sağlayamadı</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1783,14 +1783,14 @@
           <t>0 dk 55 sn</t>
         </is>
       </c>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>Çözülemedi</t>
-        </is>
-      </c>
-      <c r="F19" s="4" t="inlineStr">
-        <is>
-          <t>Pozitif</t>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>Çözüldü</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>Nötr</t>
         </is>
       </c>
       <c r="G19" s="4" t="inlineStr">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Site teknik problemi/hata</t>
+          <t>Web sitesi hatası (404 Not Found) ile ilgili bilgi talebi/şikayet</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1875,7 +1875,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Hesaplardan ödeme çekilmesi fakat sipariş görünmüyor / iade süreci ve para iadesi bekleniyor</t>
+          <t>Hesap üzerinden çekim yapılmış ancak sipariş görünmüyor/ödemeye dair sorun</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1928,9 +1928,9 @@
           <t>Çözüldü</t>
         </is>
       </c>
-      <c r="F21" s="4" t="inlineStr">
-        <is>
-          <t>Pozitif</t>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>Nötr</t>
         </is>
       </c>
       <c r="G21" s="3" t="inlineStr">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Ürün hakkında kumaş bilgisi</t>
+          <t>Ürün özelliği hakkında bilgi (kumaş niteliği)</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2015,7 +2015,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Siparişte eksik/promosyon ürünleri</t>
+          <t>Siparişte eksik/promosyon ürünlerin olması ve çözüm talebi</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>İade süreci/para iadesi gecikmesi</t>
+          <t>İade süreci gecikmesi ve para iadesi ile ilgili memnuniyetsizlik</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Kargo/hasar nedeniyle ürün hasarı bildirimi ve değişim talebi</t>
+          <t>Kargo kaynaklı hasar bildirimi ve değişim talebi</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Değişim seçeneği yok, iade+yeniden sipariş zahmetli ve memnuniyetsizlik</t>
+          <t>Değişim seçeneğinin olmaması ve iade+yeniden siparişin zahmetli oluşu</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Yanlış ürün teslimatı ve iade süreci bilgilendirmesi</t>
+          <t>Yanlış ürün gönderimi nedeniyle iade/yeniden gönderim süreci başlatıldı</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2418,9 +2418,9 @@
           <t>Çözüldü</t>
         </is>
       </c>
-      <c r="F28" s="4" t="inlineStr">
-        <is>
-          <t>Pozitif</t>
+      <c r="F28" s="3" t="inlineStr">
+        <is>
+          <t>Nötr</t>
         </is>
       </c>
       <c r="G28" s="3" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Siparişte eksik ürün ve stok hatası nedeniyle memnuniyetsizlik; iade istemiyorum, ürünün ısrarla tem</t>
+          <t>Siparişte eksik ürün ve stok hatası nedeniyle sorun yaşanıyor</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="G30" s="4" t="inlineStr">
         <is>
-          <t>Şikayet</t>
+          <t>İade</t>
         </is>
       </c>
       <c r="H30" s="3" t="inlineStr">
@@ -2575,7 +2575,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>İade süreciyle ilgili sorun ve yeni iade kodunun oluşturulması</t>
+          <t>İade süreciyle ilgili sorun çözümü ve yeni iade kodu oluşturuldu</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Teslimat adresinin yanlış yazılması ve düzeltme talebi</t>
+          <t>Teslimat adresinin yanlış yazılması ve düzeltilmesi</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2785,7 +2785,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Ödeme problemi - sipariş için ödeme işleminin gerçekleşmemesi</t>
+          <t>Hesap üzerinden ödeme çekilmemesi/tekrar deneme?</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Beden nedeniyle iade</t>
+          <t>Beden uyuşmazlığı nedeniyle iade</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="G36" s="4" t="inlineStr">
         <is>
-          <t>Şikayet</t>
+          <t>Sorun</t>
         </is>
       </c>
       <c r="H36" s="3" t="inlineStr">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Kargo takibi ve teslimat gecikmesi</t>
+          <t>Kargo takibi ve gecikme</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -3048,9 +3048,9 @@
           <t>Çözüldü</t>
         </is>
       </c>
-      <c r="F37" s="4" t="inlineStr">
-        <is>
-          <t>Nötr</t>
+      <c r="F37" s="3" t="inlineStr">
+        <is>
+          <t>Pozitif</t>
         </is>
       </c>
       <c r="G37" s="3" t="inlineStr">
@@ -3130,12 +3130,12 @@
       </c>
       <c r="H38" s="4" t="inlineStr">
         <is>
-          <t>Hasarlı ürün</t>
+          <t>Defolu ürün</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Kulaklıkta hatalı şarj sorunu ve garanti kapsamında tamir talebi</t>
+          <t>Kulaklıktaki arıza ve garanti kapsamında tamir talebi</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -3188,9 +3188,9 @@
           <t>Çözüldü</t>
         </is>
       </c>
-      <c r="F39" s="4" t="inlineStr">
-        <is>
-          <t>Pozitif</t>
+      <c r="F39" s="3" t="inlineStr">
+        <is>
+          <t>Nötr</t>
         </is>
       </c>
       <c r="G39" s="3" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Abonelikten çıkış talebi</t>
+          <t>Abonelikten çıkma talebi</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3275,7 +3275,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Kargo takibi ve teslimat gecikmesi</t>
+          <t>Kargonun gecikmesi nedeniyle teslimatın gecikmesi</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3345,7 +3345,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>İade süreci uzun sürüyor</t>
+          <t>İade süreci uzaması ve kötü hizmet</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3400,7 +3400,7 @@
         </is>
       </c>
       <c r="B46" s="6" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47">
@@ -3410,7 +3410,7 @@
         </is>
       </c>
       <c r="B47" s="6" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B48" s="6" t="inlineStr">
         <is>
-          <t>%57.5</t>
+          <t>%70.0</t>
         </is>
       </c>
     </row>

</xml_diff>